<commit_message>
Ajout de la macro recherche de zero camera. Manque l ajout du boutton
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -377,151 +377,221 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G2">
-        <f t="shared" ref="G2:G11" si="0">G3+2</f>
-        <v>32</v>
+        <f t="shared" ref="G2" si="0">G3+2</f>
+        <v>46</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H11" si="1">H3+2</f>
-        <v>31</v>
+        <f t="shared" ref="H2" si="1">H3+2</f>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G3">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f t="shared" ref="G3:G8" si="2">G4+2</f>
+        <v>44</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <f t="shared" ref="H3:H8" si="3">H4+2</f>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" si="3"/>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" si="3"/>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="3"/>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" ref="G9:G18" si="4">G10+2</f>
+        <v>32</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f>H10+2</f>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G10">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>H11+2</f>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>28</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f>H12+2</f>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G12">
-        <f>G13+2</f>
-        <v>12</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="H12">
         <f>H13+2</f>
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G13">
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="H13">
-        <v>9</v>
+        <f>H14+2</f>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G14">
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>22</v>
       </c>
       <c r="H14">
-        <v>7</v>
+        <f>H15+2</f>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G15">
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <f>H16+2</f>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G16">
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <f>H17+2</f>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G17">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <f>H18+2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <f>H19+2</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f>G20+2</f>
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <f>H20+2</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>10</v>
+      </c>
+      <c r="H20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G24">
         <v>2</v>
       </c>
-      <c r="H17">
+      <c r="H24">
         <v>1</v>
       </c>
     </row>

</xml_diff>